<commit_message>
Dream added to all ZW 2018 Grade CC1 Batch
</commit_message>
<xml_diff>
--- a/Grade 2018/Class Test/CT_Summary_ZW_2018.xlsx
+++ b/Grade 2018/Class Test/CT_Summary_ZW_2018.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repository\Sept 2020 - Jan 2021\Grade 2018\Class Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01B5BF6C-CC75-432E-9C2D-EC518DF53596}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA68A4E5-97FE-4687-B8E9-6CAE31363B83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CC1" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="461">
   <si>
     <t>Student Details</t>
   </si>
@@ -1413,6 +1413,12 @@
   </si>
   <si>
     <t>Jack  Cai</t>
+  </si>
+  <si>
+    <t>田嘉喜</t>
+  </si>
+  <si>
+    <t>Dream</t>
   </si>
 </sst>
 </file>
@@ -1917,10 +1923,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J45"/>
+  <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3037,13 +3043,13 @@
         <v>13</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>443</v>
+        <v>459</v>
       </c>
       <c r="D45" s="10">
-        <v>12017245779</v>
+        <v>12016246281</v>
       </c>
       <c r="E45" s="10" t="s">
-        <v>445</v>
+        <v>460</v>
       </c>
       <c r="F45" s="11"/>
       <c r="G45" s="11"/>
@@ -3051,6 +3057,31 @@
       <c r="I45" s="11"/>
       <c r="J45" s="12" t="e">
         <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A46" s="2">
+        <v>43</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>443</v>
+      </c>
+      <c r="D46" s="10">
+        <v>12017245779</v>
+      </c>
+      <c r="E46" s="10" t="s">
+        <v>445</v>
+      </c>
+      <c r="F46" s="11"/>
+      <c r="G46" s="11"/>
+      <c r="H46" s="11"/>
+      <c r="I46" s="11"/>
+      <c r="J46" s="12" t="e">
+        <f t="shared" ref="J46" si="2">AVERAGE(F46:I46)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -5288,8 +5319,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40:E41"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>